<commit_message>
feat: add update database initial logic
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -487,7 +487,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Arroz Diana x 1 Kilogramo</t>
+          <t>Updated Name</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -500,7 +500,7 @@
         <v>3500</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45793.57378114079</v>
+        <v>45793.57378114583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update logic for an entire row
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -487,20 +487,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Updated Name</t>
+          <t>Arroz Doña Nieves 1k</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E2" t="n">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="F2" t="n">
-        <v>3500</v>
+        <v>4500</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45793.57378114583</v>
+        <v>45793.72712263872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pruebas de guardado de datos en el archivo .xlsx
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -1,119 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="ProductData"/>
-    <sheet r:id="rId2" sheetId="2" name="categorias"/>
-    <sheet r:id="rId3" sheetId="3" name="SalesData"/>
+    <sheet name="ProductData" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="categorias" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SalesData" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>Aseo</t>
-  </si>
-  <si>
-    <t>Mercado</t>
-  </si>
-  <si>
-    <t>Alimentos</t>
-  </si>
-  <si>
-    <t>item_code</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>product_name</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>purchase_price</t>
-  </si>
-  <si>
-    <t>sale_price</t>
-  </si>
-  <si>
-    <t>creation_date</t>
-  </si>
-  <si>
-    <t>AB_001</t>
-  </si>
-  <si>
-    <t>Alimento y bebidas</t>
-  </si>
-  <si>
-    <t>Arroz Doña Nieves 1k</t>
-  </si>
-  <si>
-    <t>AB_002</t>
-  </si>
-  <si>
-    <t>Cuidado personal</t>
-  </si>
-  <si>
-    <t>Crema dental Colgate</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="4">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -151,60 +94,121 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -492,92 +496,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="3" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="8.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col width="10.43357142857143" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="18.29071428571428" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="19.86214285714286" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="8.43357142857143" bestFit="1" customWidth="1" style="4" min="4" max="4"/>
+    <col width="14.43357142857143" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
+    <col width="10.005" bestFit="1" customWidth="1" style="4" min="6" max="6"/>
+    <col width="18.14785714285714" bestFit="1" customWidth="1" style="12" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="7">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>item_code</t>
+        </is>
+      </c>
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>product_name</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="inlineStr">
+        <is>
+          <t>quantity</t>
+        </is>
+      </c>
+      <c r="E1" s="8" t="inlineStr">
+        <is>
+          <t>purchase_price</t>
+        </is>
+      </c>
+      <c r="F1" s="8" t="inlineStr">
+        <is>
+          <t>sale_price</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
+          <t>creation_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>AB_001</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Alimento y bebidas</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>Arroz Doña Nieves 1k</t>
+        </is>
+      </c>
+      <c r="D2" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="10" t="n">
         <v>3500</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="10" t="n">
         <v>4500</v>
       </c>
-      <c r="G2" s="8">
-        <v>45793.727118055554</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="G2" s="11" t="n">
+        <v>25568.79219667824</v>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>AB_002</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>Cuidado personal</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>Crema dental Colgate</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="10" t="n">
         <v>2700</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="10" t="n">
         <v>3000</v>
       </c>
-      <c r="G3" s="8">
-        <v>45794.846180555556</v>
+      <c r="G3" s="11" t="n">
+        <v>25568.79219668981</v>
       </c>
     </row>
   </sheetData>
@@ -586,37 +619,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="3" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="14.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
+    <row r="1" ht="20.25" customHeight="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>Aseo</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Mercado</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>Alimentos</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -625,16 +669,110 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="4" t="n"/>
+      <c r="B1" s="5" t="n"/>
+      <c r="C1" s="4" t="n"/>
+      <c r="D1" s="4" t="n"/>
+      <c r="E1" s="5" t="n"/>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="4" t="n"/>
+      <c r="B2" s="5" t="n"/>
+      <c r="C2" s="4" t="n"/>
+      <c r="D2" s="4" t="n"/>
+      <c r="E2" s="5" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>PRODUCTO</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>CANTIDAD</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>TOTAL  VENTA</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>FECHA DE VENTA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>Pan</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Leche</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7500</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: initialize database when running app.
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="ProductData" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CategoryData" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -487,20 +488,121 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Arroz Doña Nieves 1k</t>
+          <t>Arroz Diana x 1 Kilogramo</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="F2" t="n">
         <v>3500</v>
       </c>
-      <c r="F2" t="n">
-        <v>4500</v>
-      </c>
       <c r="G2" s="2" t="n">
-        <v>45793.72712263889</v>
+        <v>45798.88830936589</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Aseo personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Dulcería</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Limpieza</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Papelería</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Medicamentos</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: implement create code item
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,12 +478,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AB_001</t>
+          <t>1AYB</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alimento y bebidas</t>
+          <t>Alimentos y bebidas</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -501,7 +501,94 @@
         <v>3500</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45798.88830936589</v>
+        <v>45798.94746832781</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2AYB</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Aceite de oliva x 1 Litro</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>12000</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>45798.9474683279</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3AYB</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Leche Colanta x 1 litro</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3500</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>45798.94746832792</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4AYB</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Pan Integral Unidad</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>45798.94746832793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: form connected with create stock product logic and confirmation modal
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="ProductData" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CategoryData" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -430,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,7 +500,7 @@
         <v>3500</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45798.94746832781</v>
+        <v>45799.8199624074</v>
       </c>
     </row>
     <row r="3">
@@ -530,7 +529,7 @@
         <v>12000</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45798.9474683279</v>
+        <v>45799.8199624074</v>
       </c>
     </row>
     <row r="4">
@@ -559,7 +558,7 @@
         <v>3500</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>45798.94746832792</v>
+        <v>45799.8199624074</v>
       </c>
     </row>
     <row r="5">
@@ -588,108 +587,854 @@
         <v>1500</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>45798.94746832793</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Alimentos y bebidas</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+        <v>45799.8199624074</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5AYB</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Pescado en lata</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>24</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F6" t="n">
+        <v>13400</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>45799.82035740741</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6AYB</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Pescado en lata</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>24</v>
+      </c>
+      <c r="E7" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>14000</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>45799.82125142361</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7AYB</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Atun</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>24</v>
+      </c>
+      <c r="E8" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>14000</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>45799.82190545139</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1AP</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Aseo personal</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Desodorante</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>12</v>
+      </c>
+      <c r="E9" t="n">
+        <v>13000</v>
+      </c>
+      <c r="F9" t="n">
+        <v>14500</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>45799.84121640046</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>8AYB</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Jamon</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>32</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6500</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>45799.84399756944</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1D</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Dulcería</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Nerds</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>12</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4500</v>
+      </c>
+      <c r="F11" t="n">
+        <v>6000</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>45799.85411049768</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2D</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Dulcería</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Certz</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>12</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2500</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3500</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>45799.8556128588</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1P</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Papelería</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Lapiz 2 HB</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>15</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2200</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>45799.85686115741</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>9AYB</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Latisha de res</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" t="n">
+        <v>12500</v>
+      </c>
+      <c r="F14" t="n">
+        <v>16000</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>45799.85896907408</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2P</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Papelería</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Lapicero Milimetrico</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>31</v>
+      </c>
+      <c r="E15" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F15" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>45799.8602149537</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1L</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Limpieza</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Limpido Clorox</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>12</v>
+      </c>
+      <c r="E16" t="n">
+        <v>12300</v>
+      </c>
+      <c r="F16" t="n">
+        <v>15300</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>45799.86217138889</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2L</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Limpieza</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Limpido Clorox</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>12</v>
+      </c>
+      <c r="E17" t="n">
+        <v>12300</v>
+      </c>
+      <c r="F17" t="n">
+        <v>15300</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>45799.86307028935</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1M</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Medicamentos</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Formoterol x 10 pastillas</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E18" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F18" t="n">
+        <v>14500</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>45799.86403576389</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2M</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Medicamentos</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Acetaminofen x 10 pastillas Genfar</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>25</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4500</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5600</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>45799.86651685185</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>10AYB</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Sancocho empaque 200 gramos</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>22</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9800</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10500</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>45799.86766081019</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>3M</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Medicamentos</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Ibuprofeno 400 mg x 10 pastillas</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>40</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3500</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>45799.86915119213</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>11AYB</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Pollo almendrado x 500gr</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>12</v>
+      </c>
+      <c r="E22" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F22" t="n">
+        <v>14500</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>45799.87276623843</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>4M</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Medicamentos</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Cetirizina x 10 pastillas Regular</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>120</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3500</v>
+      </c>
+      <c r="F23" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>45799.87435034722</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>12AYB</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Pez Cado 12</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>12</v>
+      </c>
+      <c r="E24" t="n">
+        <v>12500</v>
+      </c>
+      <c r="F24" t="n">
+        <v>13400</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>45799.87558456018</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2AP</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Aseo personal</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Escoba Cabelluda</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>12</v>
+      </c>
+      <c r="E25" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F25" t="n">
+        <v>14000</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>45799.87664490741</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>13AYB</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Gato Asado</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>12</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F26" t="n">
+        <v>14000</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>45799.87821791667</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>14AYB</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Un pato</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>15</v>
+      </c>
+      <c r="E27" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F27" t="n">
+        <v>13000</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>45799.87950362269</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>15AYB</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Agua</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>34</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1800</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>45799.8837228125</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>16AYB</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Un prod</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>12</v>
+      </c>
+      <c r="E29" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F29" t="n">
+        <v>14000</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>45799.88586961805</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>17AYB</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Hamburguesa doble 1000gr</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>12</v>
+      </c>
+      <c r="E30" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F30" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>45799.8872652662</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>18AYB</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Nicotino</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>55</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1290</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4390</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>45799.88909518519</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>3P</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>Papelería</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Regla</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>12</v>
+      </c>
+      <c r="E32" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F32" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>45799.89002619213</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>5M</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>Medicamentos</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Otros</t>
-        </is>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Penicilina</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>45</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3400</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5600</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>45799.89237791667</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>19AYB</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Arroz Diana 1 libra</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>12000</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>1400</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>45799.89366613794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add stock search functionality and enhance stock management UI
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,7 +500,7 @@
         <v>3500</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45803.774840841</v>
+        <v>45803.7748408449</v>
       </c>
     </row>
     <row r="3">
@@ -529,7 +529,7 @@
         <v>12000</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45803.7748408411</v>
+        <v>45803.7748408449</v>
       </c>
     </row>
     <row r="4">
@@ -558,7 +558,7 @@
         <v>3500</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>45803.77484084111</v>
+        <v>45803.7748408449</v>
       </c>
     </row>
     <row r="5">
@@ -587,7 +587,42 @@
         <v>1500</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>45803.77484084112</v>
+        <v>45803.7748408449</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5AYB</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Chitos paquete grande</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>12000</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>45803.80732169651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: clean up StockCreateView by removing unused code and resetting output widget
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,23 +606,52 @@
           <t>Chitos paquete grande</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>10000</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>12000</t>
-        </is>
+      <c r="D6" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12000</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>45803.80732169651</v>
+        <v>45803.80732170139</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1P</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Papelería</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Lapicero Retractil kilometrico rojo</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1200</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>45806.85473642316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implement stock update functionality in StockCreateView and StockManageView
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -635,23 +635,81 @@
           <t>Lapicero Retractil kilometrico rojo</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2500</t>
-        </is>
+      <c r="D7" t="n">
+        <v>45</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2500</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>45806.85473642316</v>
+        <v>45806.85473642361</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1L</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Limpieza</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Limpido Clorox</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>24</v>
+      </c>
+      <c r="E8" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>16000</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>45808.66713628472</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1AP</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Aseo personal</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Jabon piel dove en barra x 4</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>5600</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>8500</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>45808.66879746068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update stock product functionality and improve notifications in StockCreateView and StockManageView
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -690,7 +690,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Jabon piel dove en barra x 4</t>
+          <t>Jabon piel dove en barra x 5</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="G9" s="2" t="n">
-        <v>45808.66879746068</v>
+        <v>45808.67727196186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: introduce StockDataRefreshMessage for improved stock data synchronization across views
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -632,20 +632,26 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Lapicero Retractil kilometrico rojo</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>45</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2500</v>
+          <t>Lapicero Retractil kilometrico azul</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1200</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
       </c>
       <c r="G7" s="2" t="n">
-        <v>45806.85473642361</v>
+        <v>45808.68072812058</v>
       </c>
     </row>
     <row r="8">
@@ -693,23 +699,17 @@
           <t>Jabon piel dove en barra x 5</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>5600</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>8500</t>
-        </is>
+      <c r="D9" t="n">
+        <v>30</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5600</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8500</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>45808.67727196186</v>
+        <v>45808.67727196759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Taskbar styles and clean unnecessary code.
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -635,23 +635,17 @@
           <t>Lapicero Retractil kilometrico azul</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2500</t>
-        </is>
+      <c r="D7" t="n">
+        <v>45</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2500</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>45808.68072812058</v>
+        <v>45808.680728125</v>
       </c>
     </row>
     <row r="8">
@@ -710,6 +704,41 @@
       </c>
       <c r="G9" s="2" t="n">
         <v>45808.67727196759</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1M</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Medicamentos</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Dolex Gripa x 12 pastillas</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>4500</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>6600</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>45810.72437689169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update stock data loading method in StockManageView to use read_stock function
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -690,7 +690,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Jabon piel dove en barra x 5</t>
+          <t>Jabon piel dove en barra x 10</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -703,7 +703,7 @@
         <v>8500</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>45808.67727196759</v>
+        <v>45813.87396958334</v>
       </c>
     </row>
     <row r="10">
@@ -719,7 +719,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dolex Gripa x 12 pastillas</t>
+          <t>Dolex Gripa x 20 pastillas</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="G10" s="2" t="n">
-        <v>45810.72437689169</v>
+        <v>45813.87414978183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: update product stock and sell data Excel files with latest changes
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -722,23 +722,52 @@
           <t>Dolex Gripa x 20 pastillas</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>4500</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>6600</t>
-        </is>
+      <c r="D10" t="n">
+        <v>50</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4500</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6600</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>45813.87414978183</v>
+        <v>45813.87414978009</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2M</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Medicamentos</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Metrotexato 1 caja 10 pastillas 200mg</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>23400</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>28000</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>45815.82747358619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implement stock update functionality in CreateSellView during sales process; enhance README with additional documentation structure and formatting improvements
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
         <v>2500</v>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E6" t="n">
         <v>10000</v>
@@ -665,7 +665,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E8" t="n">
         <v>12000</v>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E9" t="n">
         <v>5600</v>
@@ -723,7 +723,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E10" t="n">
         <v>4500</v>
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="G11" s="2" t="n">
-        <v>45815.82747358619</v>
+        <v>45818.70595449737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implement stock deletion functionality with confirmation modal in StockManageView; enhance UI for delete actions and update styles for confirmation modal
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -738,36 +738,36 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2M</t>
+          <t>2P</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Medicamentos</t>
+          <t>Papelería</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Metrotexato 1 caja 10 pastillas 200mg</t>
+          <t>Resma x 100 hojas</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>23400</t>
+          <t>10000</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>28000</t>
+          <t>15000</t>
         </is>
       </c>
       <c r="G11" s="2" t="n">
-        <v>45818.70595449737</v>
+        <v>45818.96507344174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update button label in StockCreateView to indicate edit mode; modify product stock data file
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -806,7 +806,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Micropunta 0.6mm Good lines</t>
+          <t>Micropunta 1mm Good lines</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="G13" s="2" t="n">
-        <v>45818.98101949068</v>
+        <v>45818.98260267865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: delete unnecessary files
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
         <v>2500</v>
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
         <v>2500</v>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" t="n">
         <v>10000</v>
@@ -665,7 +665,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="n">
         <v>12000</v>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9" t="n">
         <v>5600</v>
@@ -809,23 +809,52 @@
           <t>Micropunta 1mm Good lines</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2400</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>45818.98260267361</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>4P</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Papelería</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Papel Contact Pliego</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2400</t>
-        </is>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>45818.98260267865</v>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>45821.65969966252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: clean format, unused variables and comments
</commit_message>
<xml_diff>
--- a/src/business/data/product_stock_data.xlsx
+++ b/src/business/data/product_stock_data.xlsx
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
         <v>2500</v>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
         <v>8000</v>
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
         <v>1000</v>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" t="n">
         <v>10000</v>
@@ -636,7 +636,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" t="n">
         <v>1200</v>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n">
         <v>5600</v>
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="n">
         <v>10000</v>
@@ -838,23 +838,17 @@
           <t>Papel Contact Pliego</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
+      <c r="D14" t="n">
+        <v>11</v>
+      </c>
+      <c r="E14" t="n">
+        <v>400</v>
+      </c>
+      <c r="F14" t="n">
+        <v>650</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>45821.65969966252</v>
+        <v>45821.65969966435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>